<commit_message>
Added 'Deaths within 28 days...' data and charts
</commit_message>
<xml_diff>
--- a/data/deaths_within_28_days_reported.xlsx
+++ b/data/deaths_within_28_days_reported.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\githome\TTS-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6833E57-824C-45B3-A6B7-10882071DCC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561F4F31-9ACE-4B17-9FA7-CA2E913368A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="450" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_2020-Dec-06" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>reported date</t>
-  </si>
   <si>
     <t>England - Cumulative</t>
   </si>
@@ -71,13 +68,16 @@
   <si>
     <t>Wales 7 day MA per 100,000</t>
   </si>
+  <si>
+    <t>Date Notified</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -568,10 +568,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N309" sqref="N309"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,43 +940,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -14746,19 +14746,19 @@
         <v>2406</v>
       </c>
       <c r="J328" s="4">
-        <f t="shared" ref="J328:J344" si="20">SUM(B322:B328)/(7*56.287)</f>
+        <f t="shared" ref="J328:J340" si="20">SUM(B322:B328)/(7*56.287)</f>
         <v>6.7003545604288224</v>
       </c>
       <c r="K328" s="4">
-        <f t="shared" ref="K328:K344" si="21">SUM(D322:D328)/(7*1.8937)</f>
+        <f t="shared" ref="K328:K340" si="21">SUM(D322:D328)/(7*1.8937)</f>
         <v>5.2052293695637415</v>
       </c>
       <c r="L328" s="4">
-        <f t="shared" ref="L328:L344" si="22">SUM(F322:F328)/(7*5.4633)</f>
+        <f t="shared" ref="L328:L340" si="22">SUM(F322:F328)/(7*5.4633)</f>
         <v>5.7788202316234827</v>
       </c>
       <c r="M328" s="4">
-        <f t="shared" ref="M328:M344" si="23">SUM(H322:H328)/(7*3.1529)</f>
+        <f t="shared" ref="M328:M340" si="23">SUM(H322:H328)/(7*3.1529)</f>
         <v>7.4308006687720605</v>
       </c>
     </row>

</xml_diff>